<commit_message>
Working on Phonological Summary of Sentence modes in R
</commit_message>
<xml_diff>
--- a/Ch_6_Form/output/pn_by_speaker.xlsx
+++ b/Ch_6_Form/output/pn_by_speaker.xlsx
@@ -1,21 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\antoi\GitHub\PhD\Ch_6_Form\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE644985-9ECB-43EC-A71B-FCC8AADC5E43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{447E8255-5EBE-4AEF-B30E-DED31C84AA71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30855" yWindow="4230" windowWidth="12585" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="pn_by_speaker" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <externalReferences>
+    <externalReference r:id="rId2"/>
+  </externalReferences>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -604,7 +619,11 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
@@ -1186,10 +1205,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>4</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -1201,10 +1220,10 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
@@ -1330,37 +1349,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>6.1127428571428499</c:v>
+                  <c:v>6.1130000000000004</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.1247714285714201</c:v>
+                  <c:v>6.125</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.95018181818181</c:v>
+                  <c:v>4.95</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.8695277777777699</c:v>
+                  <c:v>5.87</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.02211428571428</c:v>
+                  <c:v>5.0220000000000002</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.9193437500000003</c:v>
+                  <c:v>4.9189999999999996</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5.9699032258064504</c:v>
+                  <c:v>5.97</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>6.4359142857142801</c:v>
+                  <c:v>6.4359999999999999</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>6.00621212121212</c:v>
+                  <c:v>6.0060000000000002</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>6.2629000000000001</c:v>
+                  <c:v>6.2629999999999999</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>5.6375142857142801</c:v>
+                  <c:v>5.6379999999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2367,17 +2386,263 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="pn_by_speaker"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="2">
+          <cell r="B2">
+            <v>11</v>
+          </cell>
+          <cell r="C2">
+            <v>0</v>
+          </cell>
+          <cell r="D2">
+            <v>14</v>
+          </cell>
+          <cell r="E2">
+            <v>6</v>
+          </cell>
+          <cell r="F2">
+            <v>69</v>
+          </cell>
+          <cell r="H2">
+            <v>6.1130000000000004</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="B3">
+            <v>9</v>
+          </cell>
+          <cell r="C3">
+            <v>0</v>
+          </cell>
+          <cell r="D3">
+            <v>0</v>
+          </cell>
+          <cell r="E3">
+            <v>3</v>
+          </cell>
+          <cell r="F3">
+            <v>89</v>
+          </cell>
+          <cell r="H3">
+            <v>6.125</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="B4">
+            <v>0</v>
+          </cell>
+          <cell r="C4">
+            <v>3</v>
+          </cell>
+          <cell r="D4">
+            <v>0</v>
+          </cell>
+          <cell r="E4">
+            <v>0</v>
+          </cell>
+          <cell r="F4">
+            <v>97</v>
+          </cell>
+          <cell r="H4">
+            <v>4.95</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="B5">
+            <v>0</v>
+          </cell>
+          <cell r="C5">
+            <v>0</v>
+          </cell>
+          <cell r="D5">
+            <v>6</v>
+          </cell>
+          <cell r="E5">
+            <v>6</v>
+          </cell>
+          <cell r="F5">
+            <v>89</v>
+          </cell>
+          <cell r="H5">
+            <v>5.87</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="B6">
+            <v>0</v>
+          </cell>
+          <cell r="C6">
+            <v>0</v>
+          </cell>
+          <cell r="D6">
+            <v>0</v>
+          </cell>
+          <cell r="E6">
+            <v>0</v>
+          </cell>
+          <cell r="F6">
+            <v>100</v>
+          </cell>
+          <cell r="H6">
+            <v>5.0220000000000002</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="B7">
+            <v>3</v>
+          </cell>
+          <cell r="C7">
+            <v>19</v>
+          </cell>
+          <cell r="D7">
+            <v>0</v>
+          </cell>
+          <cell r="E7">
+            <v>0</v>
+          </cell>
+          <cell r="F7">
+            <v>78</v>
+          </cell>
+          <cell r="H7">
+            <v>4.9189999999999996</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="B8">
+            <v>13</v>
+          </cell>
+          <cell r="C8">
+            <v>0</v>
+          </cell>
+          <cell r="D8">
+            <v>32</v>
+          </cell>
+          <cell r="E8">
+            <v>13</v>
+          </cell>
+          <cell r="F8">
+            <v>42</v>
+          </cell>
+          <cell r="H8">
+            <v>5.97</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="B9">
+            <v>0</v>
+          </cell>
+          <cell r="C9">
+            <v>0</v>
+          </cell>
+          <cell r="D9">
+            <v>49</v>
+          </cell>
+          <cell r="E9">
+            <v>0</v>
+          </cell>
+          <cell r="F9">
+            <v>51</v>
+          </cell>
+          <cell r="H9">
+            <v>6.4359999999999999</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="B10">
+            <v>0</v>
+          </cell>
+          <cell r="C10">
+            <v>0</v>
+          </cell>
+          <cell r="D10">
+            <v>6</v>
+          </cell>
+          <cell r="E10">
+            <v>27</v>
+          </cell>
+          <cell r="F10">
+            <v>67</v>
+          </cell>
+          <cell r="H10">
+            <v>6.0060000000000002</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="B11">
+            <v>0</v>
+          </cell>
+          <cell r="C11">
+            <v>0</v>
+          </cell>
+          <cell r="D11">
+            <v>67</v>
+          </cell>
+          <cell r="E11">
+            <v>27</v>
+          </cell>
+          <cell r="F11">
+            <v>7</v>
+          </cell>
+          <cell r="H11">
+            <v>6.2629999999999999</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="B12">
+            <v>0</v>
+          </cell>
+          <cell r="C12">
+            <v>0</v>
+          </cell>
+          <cell r="D12">
+            <v>17</v>
+          </cell>
+          <cell r="E12">
+            <v>3</v>
+          </cell>
+          <cell r="F12">
+            <v>80</v>
+          </cell>
+          <cell r="H12">
+            <v>5.6379999999999999</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="A1:G12" totalsRowShown="0">
   <autoFilter ref="A1:G12" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="speaker"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="(*)"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="L*"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="H*"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="&gt;H*"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="L*H"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="speech rate"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="(*)">
+      <calculatedColumnFormula>[1]pn_by_speaker!B2</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="L*">
+      <calculatedColumnFormula>[1]pn_by_speaker!C2</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="H*">
+      <calculatedColumnFormula>[1]pn_by_speaker!D2</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="&gt;H*">
+      <calculatedColumnFormula>[1]pn_by_speaker!E2</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="L*H">
+      <calculatedColumnFormula>[1]pn_by_speaker!F2</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="speech rate" dataDxfId="0">
+      <calculatedColumnFormula>[1]pn_by_speaker!H2</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium22" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2683,7 +2948,7 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M32" sqref="M32"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2720,22 +2985,28 @@
         <v>6</v>
       </c>
       <c r="B2">
-        <v>4</v>
+        <f>[1]pn_by_speaker!B2</f>
+        <v>11</v>
       </c>
       <c r="C2">
+        <f>[1]pn_by_speaker!C2</f>
         <v>0</v>
       </c>
       <c r="D2">
+        <f>[1]pn_by_speaker!D2</f>
         <v>14</v>
       </c>
       <c r="E2">
+        <f>[1]pn_by_speaker!E2</f>
         <v>6</v>
       </c>
       <c r="F2">
+        <f>[1]pn_by_speaker!F2</f>
         <v>69</v>
       </c>
       <c r="G2">
-        <v>6.1127428571428499</v>
+        <f>[1]pn_by_speaker!H2</f>
+        <v>6.1130000000000004</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -2743,22 +3014,28 @@
         <v>7</v>
       </c>
       <c r="B3">
+        <f>[1]pn_by_speaker!B3</f>
+        <v>9</v>
+      </c>
+      <c r="C3">
+        <f>[1]pn_by_speaker!C3</f>
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <f>[1]pn_by_speaker!D3</f>
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <f>[1]pn_by_speaker!E3</f>
         <v>3</v>
       </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <v>3</v>
-      </c>
       <c r="F3">
+        <f>[1]pn_by_speaker!F3</f>
         <v>89</v>
       </c>
       <c r="G3">
-        <v>6.1247714285714201</v>
+        <f>[1]pn_by_speaker!H3</f>
+        <v>6.125</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -2766,22 +3043,28 @@
         <v>8</v>
       </c>
       <c r="B4">
+        <f>[1]pn_by_speaker!B4</f>
         <v>0</v>
       </c>
       <c r="C4">
+        <f>[1]pn_by_speaker!C4</f>
         <v>3</v>
       </c>
       <c r="D4">
+        <f>[1]pn_by_speaker!D4</f>
         <v>0</v>
       </c>
       <c r="E4">
+        <f>[1]pn_by_speaker!E4</f>
         <v>0</v>
       </c>
       <c r="F4">
+        <f>[1]pn_by_speaker!F4</f>
         <v>97</v>
       </c>
       <c r="G4">
-        <v>4.95018181818181</v>
+        <f>[1]pn_by_speaker!H4</f>
+        <v>4.95</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -2789,22 +3072,28 @@
         <v>9</v>
       </c>
       <c r="B5">
+        <f>[1]pn_by_speaker!B5</f>
         <v>0</v>
       </c>
       <c r="C5">
+        <f>[1]pn_by_speaker!C5</f>
         <v>0</v>
       </c>
       <c r="D5">
+        <f>[1]pn_by_speaker!D5</f>
         <v>6</v>
       </c>
       <c r="E5">
+        <f>[1]pn_by_speaker!E5</f>
         <v>6</v>
       </c>
       <c r="F5">
+        <f>[1]pn_by_speaker!F5</f>
         <v>89</v>
       </c>
       <c r="G5">
-        <v>5.8695277777777699</v>
+        <f>[1]pn_by_speaker!H5</f>
+        <v>5.87</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -2812,22 +3101,28 @@
         <v>10</v>
       </c>
       <c r="B6">
+        <f>[1]pn_by_speaker!B6</f>
         <v>0</v>
       </c>
       <c r="C6">
+        <f>[1]pn_by_speaker!C6</f>
         <v>0</v>
       </c>
       <c r="D6">
+        <f>[1]pn_by_speaker!D6</f>
         <v>0</v>
       </c>
       <c r="E6">
+        <f>[1]pn_by_speaker!E6</f>
         <v>0</v>
       </c>
       <c r="F6">
+        <f>[1]pn_by_speaker!F6</f>
         <v>100</v>
       </c>
       <c r="G6">
-        <v>5.02211428571428</v>
+        <f>[1]pn_by_speaker!H6</f>
+        <v>5.0220000000000002</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -2835,22 +3130,28 @@
         <v>11</v>
       </c>
       <c r="B7">
-        <v>1</v>
+        <f>[1]pn_by_speaker!B7</f>
+        <v>3</v>
       </c>
       <c r="C7">
+        <f>[1]pn_by_speaker!C7</f>
         <v>19</v>
       </c>
       <c r="D7">
+        <f>[1]pn_by_speaker!D7</f>
         <v>0</v>
       </c>
       <c r="E7">
+        <f>[1]pn_by_speaker!E7</f>
         <v>0</v>
       </c>
       <c r="F7">
+        <f>[1]pn_by_speaker!F7</f>
         <v>78</v>
       </c>
       <c r="G7">
-        <v>4.9193437500000003</v>
+        <f>[1]pn_by_speaker!H7</f>
+        <v>4.9189999999999996</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -2858,22 +3159,28 @@
         <v>12</v>
       </c>
       <c r="B8">
-        <v>4</v>
+        <f>[1]pn_by_speaker!B8</f>
+        <v>13</v>
       </c>
       <c r="C8">
+        <f>[1]pn_by_speaker!C8</f>
         <v>0</v>
       </c>
       <c r="D8">
+        <f>[1]pn_by_speaker!D8</f>
         <v>32</v>
       </c>
       <c r="E8">
+        <f>[1]pn_by_speaker!E8</f>
         <v>13</v>
       </c>
       <c r="F8">
+        <f>[1]pn_by_speaker!F8</f>
         <v>42</v>
       </c>
       <c r="G8">
-        <v>5.9699032258064504</v>
+        <f>[1]pn_by_speaker!H8</f>
+        <v>5.97</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -2881,22 +3188,28 @@
         <v>13</v>
       </c>
       <c r="B9">
+        <f>[1]pn_by_speaker!B9</f>
         <v>0</v>
       </c>
       <c r="C9">
+        <f>[1]pn_by_speaker!C9</f>
         <v>0</v>
       </c>
       <c r="D9">
+        <f>[1]pn_by_speaker!D9</f>
         <v>49</v>
       </c>
       <c r="E9">
+        <f>[1]pn_by_speaker!E9</f>
         <v>0</v>
       </c>
       <c r="F9">
+        <f>[1]pn_by_speaker!F9</f>
         <v>51</v>
       </c>
       <c r="G9">
-        <v>6.4359142857142801</v>
+        <f>[1]pn_by_speaker!H9</f>
+        <v>6.4359999999999999</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -2904,22 +3217,28 @@
         <v>14</v>
       </c>
       <c r="B10">
+        <f>[1]pn_by_speaker!B10</f>
         <v>0</v>
       </c>
       <c r="C10">
+        <f>[1]pn_by_speaker!C10</f>
         <v>0</v>
       </c>
       <c r="D10">
+        <f>[1]pn_by_speaker!D10</f>
         <v>6</v>
       </c>
       <c r="E10">
+        <f>[1]pn_by_speaker!E10</f>
         <v>27</v>
       </c>
       <c r="F10">
+        <f>[1]pn_by_speaker!F10</f>
         <v>67</v>
       </c>
       <c r="G10">
-        <v>6.00621212121212</v>
+        <f>[1]pn_by_speaker!H10</f>
+        <v>6.0060000000000002</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -2927,22 +3246,28 @@
         <v>15</v>
       </c>
       <c r="B11">
+        <f>[1]pn_by_speaker!B11</f>
         <v>0</v>
       </c>
       <c r="C11">
+        <f>[1]pn_by_speaker!C11</f>
         <v>0</v>
       </c>
       <c r="D11">
+        <f>[1]pn_by_speaker!D11</f>
         <v>67</v>
       </c>
       <c r="E11">
+        <f>[1]pn_by_speaker!E11</f>
         <v>27</v>
       </c>
       <c r="F11">
+        <f>[1]pn_by_speaker!F11</f>
         <v>7</v>
       </c>
       <c r="G11">
-        <v>6.2629000000000001</v>
+        <f>[1]pn_by_speaker!H11</f>
+        <v>6.2629999999999999</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -2950,22 +3275,28 @@
         <v>16</v>
       </c>
       <c r="B12">
+        <f>[1]pn_by_speaker!B12</f>
         <v>0</v>
       </c>
       <c r="C12">
+        <f>[1]pn_by_speaker!C12</f>
         <v>0</v>
       </c>
       <c r="D12">
+        <f>[1]pn_by_speaker!D12</f>
         <v>17</v>
       </c>
       <c r="E12">
+        <f>[1]pn_by_speaker!E12</f>
         <v>3</v>
       </c>
       <c r="F12">
+        <f>[1]pn_by_speaker!F12</f>
         <v>80</v>
       </c>
       <c r="G12">
-        <v>5.6375142857142801</v>
+        <f>[1]pn_by_speaker!H12</f>
+        <v>5.6379999999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>